<commit_message>
Added sockets to BOM
</commit_message>
<xml_diff>
--- a/Replika/BOM/mistrum_final_BOM.xlsx
+++ b/Replika/BOM/mistrum_final_BOM.xlsx
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D34" authorId="0">
+    <comment ref="D35" authorId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="0">
+    <comment ref="D40" authorId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D92" authorId="0">
+    <comment ref="D99" authorId="0">
       <text>
         <r>
           <rPr>
@@ -104,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D93" authorId="0">
+    <comment ref="D100" authorId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G70" authorId="0">
+    <comment ref="G77" authorId="0">
       <text>
         <r>
           <rPr>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="441">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -371,7 +371,7 @@
     <t xml:space="preserve">810-CC45SL3AD100JYNA</t>
   </si>
   <si>
-    <t xml:space="preserve">C201, C202, C203, C204, C205</t>
+    <t xml:space="preserve">C201, C202, C203</t>
   </si>
   <si>
     <t xml:space="preserve">Tantal RM 5mm/Axial 10mm</t>
@@ -389,7 +389,7 @@
     <t xml:space="preserve">filtračné kondenzátory, pájkovať priamo na napájací rozvod</t>
   </si>
   <si>
-    <t xml:space="preserve">C206, C207, C208, C209, C210, C211, C212, C213, C214, C215, C216, C217, C218, C219, C220</t>
+    <t xml:space="preserve">C206, C207, C208, C209, C210, C211, C212, C213, C214, C215, C216, C217, C218, C219, C220, C221, C222, C223, C224, C225, C226, C227, C228, C229, C230</t>
   </si>
   <si>
     <t xml:space="preserve">D1, D3, D4, D5, D6, D7, D8, D9, D10</t>
@@ -494,6 +494,24 @@
     <t xml:space="preserve">UA880D</t>
   </si>
   <si>
+    <t xml:space="preserve">*IO13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket DIP-40 15.24mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICVT-40P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">649-DILB40P223TLF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objimka 40 pin</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO15, IO47, IO73, IO82, IO102</t>
   </si>
   <si>
@@ -623,6 +641,24 @@
     <t xml:space="preserve">DIP-28_W15.24mm</t>
   </si>
   <si>
+    <t xml:space="preserve">*IO42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket DIP-28 15.24mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30610</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICVT-28P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">649-DILB28P223TLF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objimka 28 pin</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO43, IO45, IO46</t>
   </si>
   <si>
@@ -635,6 +671,21 @@
     <t xml:space="preserve">MHB4164, K565RU5</t>
   </si>
   <si>
+    <t xml:space="preserve">*IO51, *IO61, *IO71, *IO81, *IO91, *IO101, *IO111, *IO121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket DIP-16 7.62mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30605</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICVT-16P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objimka 16 pin</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO52</t>
   </si>
   <si>
@@ -642,6 +693,9 @@
   </si>
   <si>
     <t xml:space="preserve">MH74S571</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*IO52</t>
   </si>
   <si>
     <t xml:space="preserve">IO53, IO54, IO55, IO56, IO57, IO67</t>
@@ -731,6 +785,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">74LS295</t>
     </r>
@@ -751,13 +806,34 @@
     <t xml:space="preserve">osadiť buď 6264 alebo 4x6116 +IO115</t>
   </si>
   <si>
+    <t xml:space="preserve">*IO77</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO77, IO97, IO117, IO127</t>
   </si>
   <si>
     <t xml:space="preserve">DIP-24_W15.24mm</t>
   </si>
   <si>
-    <t xml:space="preserve">K537RU10, 6116, 2kx8 DIP24</t>
+    <t xml:space="preserve">K537RU10, 6116, 2kx8 DIP24, 150ns+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*IO97, *IO117, *IO127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket DIP-24 15.24mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30609</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICVT-24P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">649-DILB24P-223TLF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objimka 24 pin</t>
   </si>
   <si>
     <t xml:space="preserve">IO83</t>
@@ -808,6 +884,9 @@
     <t xml:space="preserve">MH74188</t>
   </si>
   <si>
+    <t xml:space="preserve">*IO113</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO114</t>
   </si>
   <si>
@@ -925,23 +1004,7 @@
     <t xml:space="preserve">lubovoľné 5mm LED červená+zelená</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">P1, P3, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">P4, P5, P6</t>
-    </r>
+    <t xml:space="preserve">P1, P3, P4, P5, P6</t>
   </si>
   <si>
     <t xml:space="preserve">PinHeader_1x01_P2.54mm_Vertical</t>
@@ -977,23 +1040,7 @@
     <t xml:space="preserve">TR191, TR213, MLT0.25 (ľubovoľný 0.25W rezistor)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">R3, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">R37, R61, R100</t>
-    </r>
+    <t xml:space="preserve">R3, R37, R61, R100</t>
   </si>
   <si>
     <t xml:space="preserve">100R</t>
@@ -1008,23 +1055,7 @@
     <t xml:space="preserve">71-CCF07100RJKE36</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">R4, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">R30, R33, R58, R68, R77</t>
-    </r>
+    <t xml:space="preserve">R4, R30, R33, R58, R68, R77</t>
   </si>
   <si>
     <t xml:space="preserve">680R</t>
@@ -1054,32 +1085,7 @@
     <t xml:space="preserve">71-CCF075K60JKE36</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">R8, R9, R10, R11, R12, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">R38, R39, R42, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">R66</t>
-    </r>
+    <t xml:space="preserve">R8, R9, R10, R11, R12, R38, R39, R42, R66</t>
   </si>
   <si>
     <t xml:space="preserve">4K7</t>
@@ -1121,32 +1127,7 @@
     <t xml:space="preserve">71-CCF0733R0JKE36</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">R26, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">R27, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">R28, R46, R47, R48, R49, R93</t>
-    </r>
+    <t xml:space="preserve">R26, R27, R28, R46, R47, R48, R49, R93</t>
   </si>
   <si>
     <t xml:space="preserve">3K3</t>
@@ -1161,49 +1142,7 @@
     <t xml:space="preserve">71-CCF073K30JKE36</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">R32, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">R44, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">R50, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">R60, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">R62, R64, R65, R91, R92</t>
-    </r>
+    <t xml:space="preserve">R32, R44, R50, R60, R62, R64, R65, R91, R92</t>
   </si>
   <si>
     <t xml:space="preserve">1K</t>
@@ -1482,25 +1421,7 @@
     <t xml:space="preserve">SPEAKER</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">pin header, repro odporucam Mouser </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">497-SM230332-1</t>
-    </r>
+    <t xml:space="preserve">pin header, repro odporucam Mouser 497-SM230332-1</t>
   </si>
   <si>
     <t xml:space="preserve">SW2, SW1</t>
@@ -1554,25 +1475,7 @@
     <t xml:space="preserve">14MHz</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">jediny zdroj, o ktorom viem, je Farnell </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">9509488</t>
-    </r>
+    <t xml:space="preserve">jediny zdroj, o ktorom viem, je Farnell 9509488</t>
   </si>
 </sst>
 </file>
@@ -1582,7 +1485,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1617,17 +1520,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1685,7 +1577,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1714,12 +1606,8 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1803,18 +1691,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E58" activeCellId="0" sqref="E58"/>
+      <selection pane="bottomLeft" activeCell="A115" activeCellId="0" sqref="A115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="21.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.17"/>
@@ -2168,7 +2056,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>78</v>
       </c>
@@ -2176,7 +2064,7 @@
         <v>79</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>80</v>
@@ -2194,7 +2082,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>84</v>
       </c>
@@ -2202,7 +2090,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>47</v>
@@ -2387,113 +2275,111 @@
         <v>119</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="C26" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E26" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="F26" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C27" s="3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C28" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C29" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C30" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>140</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="E30" s="3"/>
       <c r="F30" s="4" t="s">
         <v>141</v>
       </c>
@@ -2509,15 +2395,17 @@
         <v>144</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C31" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="E31" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="E31" s="3"/>
       <c r="F31" s="4" t="s">
         <v>147</v>
       </c>
@@ -2533,37 +2421,37 @@
         <v>150</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C32" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C33" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="4" t="s">
@@ -2584,227 +2472,226 @@
         <v>161</v>
       </c>
       <c r="C34" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D34" s="5" t="n">
-        <v>27128</v>
+        <v>4</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
+      <c r="F34" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>164</v>
+      </c>
       <c r="H34" s="0" t="s">
-        <v>88</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="C35" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D35" s="5" t="n">
-        <v>8282</v>
+        <v>27128</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="0" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="C36" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="D36" s="5" t="n">
-        <v>4164</v>
-      </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>172</v>
+      </c>
       <c r="H36" s="0" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="C37" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>167</v>
+        <v>3</v>
+      </c>
+      <c r="D37" s="5" t="n">
+        <v>8282</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C38" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>170</v>
+        <v>8</v>
+      </c>
+      <c r="D38" s="5" t="n">
+        <v>4164</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="4" t="s">
-        <v>171</v>
-      </c>
+      <c r="G38" s="3"/>
       <c r="H38" s="0" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="C39" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D39" s="5" t="n">
-        <v>8286</v>
-      </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>181</v>
+      </c>
       <c r="G39" s="3"/>
       <c r="H39" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C40" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E40" s="3"/>
-      <c r="F40" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>178</v>
-      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
       <c r="H40" s="0" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C41" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D41" s="5" t="s">
+      <c r="F41" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="4" t="s">
+      <c r="G41" s="3"/>
+      <c r="H41" s="0" t="s">
         <v>182</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="H41" s="0" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="C42" s="3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E42" s="3"/>
-      <c r="F42" s="4" t="s">
-        <v>187</v>
-      </c>
+      <c r="F42" s="3"/>
       <c r="G42" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>103</v>
+        <v>161</v>
       </c>
       <c r="C43" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>191</v>
+        <v>1</v>
+      </c>
+      <c r="D43" s="5" t="n">
+        <v>8286</v>
       </c>
       <c r="E43" s="3"/>
-      <c r="F43" s="4" t="s">
-        <v>192</v>
-      </c>
+      <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+      <c r="B44" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B44" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="C44" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D44" s="6" t="n">
-        <v>6164</v>
-      </c>
+      <c r="E44" s="3"/>
       <c r="F44" s="4" t="s">
         <v>195</v>
       </c>
@@ -2814,88 +2701,89 @@
       <c r="H44" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="I44" s="7" t="s">
-        <v>198</v>
-      </c>
     </row>
     <row r="45" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="E45" s="3"/>
+      <c r="F45" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C45" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D45" s="6" t="n">
-        <v>6116</v>
+      <c r="G45" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="I45" s="7"/>
+        <v>202</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B46" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>203</v>
-      </c>
+      <c r="C46" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E46" s="3"/>
       <c r="F46" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="I46" s="7"/>
+        <v>207</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="C47" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D47" s="6" t="s">
         <v>208</v>
       </c>
+      <c r="B47" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E47" s="3"/>
       <c r="F47" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>209</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="G47" s="3"/>
       <c r="H47" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="I47" s="7"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>212</v>
+        <v>1</v>
+      </c>
+      <c r="D48" s="6" t="n">
+        <v>6164</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>213</v>
@@ -2906,962 +2794,1126 @@
       <c r="H48" s="0" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I48" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>145</v>
+        <v>217</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D49" s="6" t="n">
-        <v>74188</v>
+      <c r="D49" s="6"/>
+      <c r="E49" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>173</v>
+      </c>
+      <c r="I49" s="7"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>145</v>
+        <v>219</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="G50" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="6" t="n">
+        <v>6116</v>
+      </c>
+      <c r="H50" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="H50" s="0" t="s">
-        <v>221</v>
-      </c>
+      <c r="I50" s="7"/>
     </row>
     <row r="51" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B51" s="0" t="s">
-        <v>103</v>
-      </c>
       <c r="C51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D51" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" s="4" t="s">
         <v>223</v>
       </c>
+      <c r="F51" s="4" t="s">
+        <v>224</v>
+      </c>
       <c r="G51" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>226</v>
+      </c>
+      <c r="I51" s="7"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>103</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D52" s="6" t="n">
-        <v>4066</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>227</v>
+        <v>1</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>231</v>
+      </c>
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>232</v>
+        <v>151</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>233</v>
       </c>
+      <c r="F53" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>234</v>
+      </c>
       <c r="H53" s="0" t="s">
-        <v>234</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="I53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>236</v>
+        <v>237</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>239</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>239</v>
+        <v>151</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>239</v>
+        <v>1</v>
+      </c>
+      <c r="D55" s="6" t="n">
+        <v>74188</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="C56" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D56" s="6" t="s">
         <v>243</v>
       </c>
+      <c r="B56" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" s="5"/>
       <c r="E56" s="4" t="s">
-        <v>244</v>
+        <v>180</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>246</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="G56" s="3"/>
       <c r="H56" s="0" t="s">
-        <v>247</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>151</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="4" t="s">
-        <v>249</v>
+      <c r="D57" s="6" t="s">
+        <v>245</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="H58" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D59" s="6" t="n">
+        <v>4066</v>
+      </c>
+      <c r="E59" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="F59" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C58" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D58" s="6" t="s">
+      <c r="G59" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="H58" s="0" t="s">
+      <c r="H59" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="8" t="s">
+    <row r="60" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="B59" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="C59" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="H59" s="0" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2" t="s">
-        <v>260</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>258</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D60" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="H60" s="0" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
+      <c r="B61" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="C61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="H61" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="C61" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="D61" s="6" t="s">
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="B62" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="F61" s="4" t="s">
+      <c r="C62" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="H62" s="0" t="s">
         <v>266</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="H61" s="0" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C62" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="G62" s="9" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>263</v>
+        <v>267</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>268</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>278</v>
+        <v>272</v>
+      </c>
+      <c r="H63" s="0" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D64" s="6" t="s">
-        <v>280</v>
-      </c>
+      <c r="D64" s="6"/>
       <c r="E64" s="4" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>283</v>
+        <v>277</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>263</v>
+        <v>279</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>280</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>287</v>
+        <v>281</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H67" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C66" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D66" s="6" t="s">
+      <c r="B68" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="C68" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D68" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="F66" s="4" t="s">
+      <c r="E68" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="G66" s="4" t="s">
+      <c r="F68" s="4" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="s">
+      <c r="G68" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C67" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D67" s="6" t="s">
+      <c r="H68" s="0" t="s">
         <v>294</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C68" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>304</v>
+        <v>296</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>297</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>306</v>
+        <v>298</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>333</v>
+        <v>325</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>326</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C78" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C81" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>362</v>
+        <v>354</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>355</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C85" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="B86" s="0" t="s">
-        <v>386</v>
+        <v>377</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>289</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>387</v>
+        <v>378</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>379</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="B87" s="0" t="s">
-        <v>391</v>
+        <v>382</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>289</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>289</v>
+        <v>383</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>384</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>392</v>
+        <v>385</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="B88" s="0" t="s">
-        <v>394</v>
+        <v>387</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>289</v>
       </c>
       <c r="C88" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="H88" s="0" t="s">
-        <v>396</v>
+        <v>388</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D90" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="B89" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="C89" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D89" s="6" t="s">
+      <c r="E90" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="H89" s="0" t="s">
+      <c r="F90" s="4" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="2" t="s">
+      <c r="G90" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="B90" s="0" t="s">
+    </row>
+    <row r="91" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="C90" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D90" s="6" t="s">
+      <c r="B91" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D91" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="H90" s="0" t="s">
+      <c r="E91" s="4" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="2" t="s">
+      <c r="F91" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="B91" s="0" t="s">
+      <c r="G91" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="C91" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D91" s="6" t="s">
+    </row>
+    <row r="92" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="H91" s="0" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="2" t="s">
+      <c r="B92" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D92" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="B92" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="C92" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D92" s="6" t="s">
+      <c r="E92" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="H92" s="0" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F92" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>410</v>
-      </c>
-      <c r="H93" s="0" t="s">
-        <v>403</v>
+        <v>413</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="C94" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>413</v>
-      </c>
-      <c r="H94" s="0" t="s">
-        <v>414</v>
+        <v>315</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="H96" s="0" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="H97" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="H98" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="H99" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="H100" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -3871,7 +3923,7 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I44:I47"/>
+    <mergeCell ref="I48:I53"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId2" display="15804S"/>
@@ -3885,43 +3937,43 @@
     <hyperlink ref="G5" r:id="rId10" display="594-F151K25Y5RN63J5R"/>
     <hyperlink ref="F6" r:id="rId11" display="CC-271/500"/>
     <hyperlink ref="G6" r:id="rId12" display="594-D271K20Y5PH63L6R"/>
-    <hyperlink ref="E7" r:id="rId13" location="" display="117698"/>
+    <hyperlink ref="E7" r:id="rId13" display="117698"/>
     <hyperlink ref="F7" r:id="rId14" display="CC-27"/>
     <hyperlink ref="G7" r:id="rId15" display="810-CC45SL3AD270JYNA"/>
     <hyperlink ref="F8" r:id="rId16" display="CM-150N"/>
     <hyperlink ref="G8" r:id="rId17" display="810-FA28X7R1H154KRU6"/>
-    <hyperlink ref="E9" r:id="rId18" location="" display="117698"/>
+    <hyperlink ref="E9" r:id="rId18" display="117698"/>
     <hyperlink ref="F9" r:id="rId19" display="CC-27"/>
     <hyperlink ref="G9" r:id="rId20" display="810-CC45SL3AD270JYNA"/>
     <hyperlink ref="F10" r:id="rId21" display="JFGC-0.22U/250"/>
     <hyperlink ref="G10" r:id="rId22" display="598-224MWR100K"/>
-    <hyperlink ref="E11" r:id="rId23" location="" display="25034"/>
+    <hyperlink ref="E11" r:id="rId23" display="25034"/>
     <hyperlink ref="F11" r:id="rId24" display="CC-104/100"/>
     <hyperlink ref="G11" r:id="rId25" display="594-K104M15X7RF53H5"/>
-    <hyperlink ref="E12" r:id="rId26" location="" display="15715"/>
+    <hyperlink ref="E12" r:id="rId26" display="15715"/>
     <hyperlink ref="G12" r:id="rId27" display="598-477TTA016M"/>
-    <hyperlink ref="E13" r:id="rId28" location="" display="343361"/>
+    <hyperlink ref="E13" r:id="rId28" display="343361"/>
     <hyperlink ref="F13" r:id="rId29" display="CC-1N"/>
     <hyperlink ref="G13" r:id="rId30" display="594-D102K20Y5PH63L2R"/>
-    <hyperlink ref="E14" r:id="rId31" location="" display="56218"/>
+    <hyperlink ref="E14" r:id="rId31" display="56218"/>
     <hyperlink ref="F14" r:id="rId32" display="CC-681/100"/>
     <hyperlink ref="G14" r:id="rId33" display="594-D681K20Y5PH63J5R"/>
-    <hyperlink ref="E15" r:id="rId34" location="" display="56209"/>
+    <hyperlink ref="E15" r:id="rId34" display="56209"/>
     <hyperlink ref="F15" r:id="rId35" display="CC-33/100"/>
     <hyperlink ref="G15" r:id="rId36" display="810-CC45SL3AD330JYNA"/>
-    <hyperlink ref="E16" r:id="rId37" location="" display="56206"/>
+    <hyperlink ref="E16" r:id="rId37" display="56206"/>
     <hyperlink ref="F16" r:id="rId38" display="CC-10/100"/>
     <hyperlink ref="G16" r:id="rId39" display="810-CC45SL3AD100JYNA"/>
-    <hyperlink ref="E17" r:id="rId40" location="" display="15802"/>
+    <hyperlink ref="E17" r:id="rId40" display="15802"/>
     <hyperlink ref="F17" r:id="rId41" display="TC-47/6.3"/>
     <hyperlink ref="G17" r:id="rId42" display="74-173D226X9006WE3"/>
-    <hyperlink ref="E18" r:id="rId43" location="" display="25034"/>
+    <hyperlink ref="E18" r:id="rId43" display="25034"/>
     <hyperlink ref="F18" r:id="rId44" display="CC-104/100"/>
     <hyperlink ref="G18" r:id="rId45" display="594-K104M15X7RF53H5"/>
-    <hyperlink ref="E21" r:id="rId46" location="" display="14167"/>
+    <hyperlink ref="E21" r:id="rId46" display="14167"/>
     <hyperlink ref="F21" r:id="rId47" display="BZX55C3V0-YAN"/>
     <hyperlink ref="G21" r:id="rId48" display="771-BZX79-C3V0113"/>
-    <hyperlink ref="E22" r:id="rId49" location="" display="16258"/>
+    <hyperlink ref="E22" r:id="rId49" display="16258"/>
     <hyperlink ref="G22" r:id="rId50" display="774-2084"/>
     <hyperlink ref="F23" r:id="rId51" display="SN74LS04N"/>
     <hyperlink ref="G23" r:id="rId52" display="595-SN74LS04N"/>
@@ -3929,127 +3981,145 @@
     <hyperlink ref="G24" r:id="rId54" display="595-SN74LS14NE4"/>
     <hyperlink ref="F25" r:id="rId55" display="Z84C2006PEG"/>
     <hyperlink ref="G25" r:id="rId56" display="692-Z84C0006PEG"/>
-    <hyperlink ref="F26" r:id="rId57" display="SN74LS74AN"/>
-    <hyperlink ref="G26" r:id="rId58" display="595-SN74LS74AN"/>
-    <hyperlink ref="F27" r:id="rId59" display="SN74LS125AN"/>
-    <hyperlink ref="G27" r:id="rId60" display="595-SN74LS125AN"/>
-    <hyperlink ref="F28" r:id="rId61" display="SN74LS32N"/>
-    <hyperlink ref="G28" r:id="rId62" display="595-SN74LS32N"/>
-    <hyperlink ref="F29" r:id="rId63" display="74LS08"/>
-    <hyperlink ref="G29" r:id="rId64" display="595-SN74LS08N"/>
-    <hyperlink ref="E30" r:id="rId65" location="" display="26556"/>
-    <hyperlink ref="F30" r:id="rId66" display="SN74LS00N"/>
-    <hyperlink ref="G30" r:id="rId67" display="595-SN74LS00N"/>
-    <hyperlink ref="F31" r:id="rId68" display="SN74LS123N"/>
-    <hyperlink ref="G31" r:id="rId69" display="595-SN74LS123N"/>
-    <hyperlink ref="F32" r:id="rId70" display="74LS157"/>
-    <hyperlink ref="G32" r:id="rId71" display="595-SN74LS157N"/>
-    <hyperlink ref="F33" r:id="rId72" display="SN74LS245N"/>
-    <hyperlink ref="G33" r:id="rId73" display="595-SN74LS245N"/>
-    <hyperlink ref="G38" r:id="rId74" display="595-SN74LS193N"/>
-    <hyperlink ref="F40" r:id="rId75" display="NTE74LS257"/>
-    <hyperlink ref="G40" r:id="rId76" display="595-SN74LS257BN"/>
-    <hyperlink ref="F41" r:id="rId77" display="SN74LS138N"/>
-    <hyperlink ref="G41" r:id="rId78" display="595-SN74LS138N"/>
-    <hyperlink ref="F42" r:id="rId79" display="NTE74LS86"/>
-    <hyperlink ref="G42" r:id="rId80" display="595-SN74LS86AN"/>
-    <hyperlink ref="F43" r:id="rId81" display="NTE74LS95B"/>
-    <hyperlink ref="F44" r:id="rId82" display="AS6C6264-55PIN"/>
-    <hyperlink ref="G44" r:id="rId83" display="913-AS6C6264-55PCN"/>
-    <hyperlink ref="F46" r:id="rId84" display="SN74LS20N"/>
-    <hyperlink ref="G46" r:id="rId85" display="595-SN74LS20N"/>
-    <hyperlink ref="F47" r:id="rId86" display="74LS175"/>
-    <hyperlink ref="G47" r:id="rId87" display="595-SN74LS175N"/>
-    <hyperlink ref="F48" r:id="rId88" display="SN74LS153N"/>
-    <hyperlink ref="G48" r:id="rId89" display="595-SN74LS153N"/>
-    <hyperlink ref="F50" r:id="rId90" display="74LS174"/>
-    <hyperlink ref="G50" r:id="rId91" display="595-SN74LS174N"/>
-    <hyperlink ref="G51" r:id="rId92" display="595-SN74S04N"/>
-    <hyperlink ref="E52" r:id="rId93" location="" display="17539"/>
-    <hyperlink ref="F52" r:id="rId94" display="SN74HC4066N"/>
-    <hyperlink ref="G52" r:id="rId95" display="595-CD4066BE"/>
-    <hyperlink ref="E56" r:id="rId96" location="" display="19226"/>
-    <hyperlink ref="F56" r:id="rId97" display="DSC-025"/>
-    <hyperlink ref="G56" r:id="rId98" display="710-61802524823"/>
-    <hyperlink ref="E57" r:id="rId99" location="" display="28738"/>
-    <hyperlink ref="F57" r:id="rId100" display="DLA10-N"/>
-    <hyperlink ref="G57" r:id="rId101" display="652-78F100J-TR-RC"/>
-    <hyperlink ref="E61" r:id="rId102" location="" display="30981"/>
-    <hyperlink ref="F61" r:id="rId103" display="CF1/4W-10K"/>
-    <hyperlink ref="G61" r:id="rId104" display="71-CCF0710K0JKE36"/>
-    <hyperlink ref="E62" r:id="rId105" location="" display="30753"/>
-    <hyperlink ref="F62" r:id="rId106" display="CF1/4W-100R"/>
-    <hyperlink ref="G62" r:id="rId107" display="71-CCF07100RJKE36"/>
-    <hyperlink ref="E63" r:id="rId108" location="" display="30848"/>
-    <hyperlink ref="F63" r:id="rId109" display="CF1/4W-680R"/>
-    <hyperlink ref="G63" r:id="rId110" display="71-CCF07680RJKE36"/>
-    <hyperlink ref="E64" r:id="rId111" location="" display="30952"/>
-    <hyperlink ref="F64" r:id="rId112" display="CF1/4W-5K6"/>
-    <hyperlink ref="G64" r:id="rId113" display="71-CCF075K60JKE36"/>
-    <hyperlink ref="F65" r:id="rId114" display="CF1/4W-4K7"/>
-    <hyperlink ref="G65" r:id="rId115" display="71-CCF07-J-4.7K-E3"/>
-    <hyperlink ref="E66" r:id="rId116" location="" display="30789"/>
-    <hyperlink ref="F66" r:id="rId117" display="CF1/4W-220R"/>
-    <hyperlink ref="G66" r:id="rId118" display="71-CCF07220RJKE36"/>
-    <hyperlink ref="E67" r:id="rId119" location="" display="30696"/>
-    <hyperlink ref="F67" r:id="rId120" display="CF1/4W-33R"/>
-    <hyperlink ref="G67" r:id="rId121" display="71-CCF0733R0JKE36"/>
-    <hyperlink ref="E68" r:id="rId122" location="" display="30924"/>
-    <hyperlink ref="F68" r:id="rId123" display="CF1/4W-3K3"/>
-    <hyperlink ref="G68" r:id="rId124" display="71-CCF073K30JKE36"/>
-    <hyperlink ref="F69" r:id="rId125" display="CF1/4W-1K"/>
-    <hyperlink ref="G69" r:id="rId126" display="71-CCF071K00JKE36"/>
-    <hyperlink ref="E70" r:id="rId127" location="" display="30780"/>
-    <hyperlink ref="F70" r:id="rId128" display="CF1/4W-180R"/>
-    <hyperlink ref="G70" r:id="rId129" display="71-CCF07160RJKE36"/>
-    <hyperlink ref="E71" r:id="rId130" location="" display="30933"/>
-    <hyperlink ref="F71" r:id="rId131" display="CF1/4W-3K9"/>
-    <hyperlink ref="G71" r:id="rId132" display="603-CFR-25JB-52-3K9"/>
-    <hyperlink ref="E72" r:id="rId133" location="" display="30829"/>
-    <hyperlink ref="F72" r:id="rId134" display="CF1/4W-470R"/>
-    <hyperlink ref="G72" r:id="rId135" display="71-CCF07470RJKE36"/>
-    <hyperlink ref="E73" r:id="rId136" location="" display="30999"/>
-    <hyperlink ref="F73" r:id="rId137" display="CF1/4W-15K"/>
-    <hyperlink ref="G73" r:id="rId138" display="71-CCF0715K0JKE36"/>
-    <hyperlink ref="E74" r:id="rId139" location="" display="30800"/>
-    <hyperlink ref="F74" r:id="rId140" display="CF1/4W-270R"/>
-    <hyperlink ref="G74" r:id="rId141" display="603-CFR-25JB-52-270R"/>
-    <hyperlink ref="F75" r:id="rId142" display="CF1/4W-2K2"/>
-    <hyperlink ref="G75" r:id="rId143" display="71-CCF072K20JKE36"/>
-    <hyperlink ref="E76" r:id="rId144" location="" display="30871"/>
-    <hyperlink ref="F76" r:id="rId145" display="CF1/4W-1K1"/>
-    <hyperlink ref="G76" r:id="rId146" display="603-CFR-25JR-52-1K1"/>
-    <hyperlink ref="E77" r:id="rId147" location="" display="30734"/>
-    <hyperlink ref="F77" r:id="rId148" display="CF1/4W-68R"/>
-    <hyperlink ref="G77" r:id="rId149" display="71-CCF0768R0JKE36"/>
-    <hyperlink ref="E78" r:id="rId150" location="" display="31028"/>
-    <hyperlink ref="F78" r:id="rId151" display="CF1/4W-27K"/>
-    <hyperlink ref="G78" r:id="rId152" display="603-CFR-25JB-52-27K"/>
-    <hyperlink ref="E79" r:id="rId153" location="" display="30810"/>
-    <hyperlink ref="F79" r:id="rId154" display="CF1/4W-330R"/>
-    <hyperlink ref="G79" r:id="rId155" display="71-CCF07330RJKE36"/>
-    <hyperlink ref="E80" r:id="rId156" location="" display="30857"/>
-    <hyperlink ref="F80" r:id="rId157" display="CF1/4W-820R"/>
-    <hyperlink ref="G80" r:id="rId158" display="71-CCF07820RJKE36"/>
-    <hyperlink ref="F81" r:id="rId159" display="CF1/4W-22R"/>
-    <hyperlink ref="G81" r:id="rId160" display="71-CCF0722R0JKE36"/>
-    <hyperlink ref="E82" r:id="rId161" location="" display="31038"/>
-    <hyperlink ref="F82" r:id="rId162" display="CF1/4W-33K"/>
-    <hyperlink ref="G82" r:id="rId163" display="71-CCF0733K0JKE36"/>
-    <hyperlink ref="E83" r:id="rId164" location="" display="30875"/>
-    <hyperlink ref="F83" r:id="rId165" display="CF1/4W-1K2"/>
-    <hyperlink ref="G83" r:id="rId166" display="603-CFR-25JR-521K2"/>
-    <hyperlink ref="E84" r:id="rId167" location="" display="31209"/>
-    <hyperlink ref="F84" r:id="rId168" display="CF1/4W-1M"/>
-    <hyperlink ref="G84" r:id="rId169" display="71-CCF071M00JKE36"/>
-    <hyperlink ref="E85" r:id="rId170" location="" display="30819"/>
-    <hyperlink ref="F85" r:id="rId171" display="CF1/4W-390R"/>
-    <hyperlink ref="G85" r:id="rId172" display="71-CCF07390RJKE36"/>
-    <hyperlink ref="F86" r:id="rId173" display="4609X-101-102LF"/>
-    <hyperlink ref="G86" r:id="rId174" display="652-4609X-1LF-10K"/>
-    <hyperlink ref="F87" r:id="rId175" display="CA6H-250"/>
-    <hyperlink ref="H88" r:id="rId176" display="497-SM230332-1"/>
-    <hyperlink ref="H94" r:id="rId177" display="9509488"/>
+    <hyperlink ref="E26" r:id="rId57" location="" display="30612"/>
+    <hyperlink ref="F26" r:id="rId58" display="ICVT-40P"/>
+    <hyperlink ref="G26" r:id="rId59" display="649-DILB40P223TLF"/>
+    <hyperlink ref="F27" r:id="rId60" display="SN74LS74AN"/>
+    <hyperlink ref="G27" r:id="rId61" display="595-SN74LS74AN"/>
+    <hyperlink ref="F28" r:id="rId62" display="SN74LS125AN"/>
+    <hyperlink ref="G28" r:id="rId63" display="595-SN74LS125AN"/>
+    <hyperlink ref="F29" r:id="rId64" display="SN74LS32N"/>
+    <hyperlink ref="G29" r:id="rId65" display="595-SN74LS32N"/>
+    <hyperlink ref="F30" r:id="rId66" display="74LS08"/>
+    <hyperlink ref="G30" r:id="rId67" display="595-SN74LS08N"/>
+    <hyperlink ref="E31" r:id="rId68" display="26556"/>
+    <hyperlink ref="F31" r:id="rId69" display="SN74LS00N"/>
+    <hyperlink ref="G31" r:id="rId70" display="595-SN74LS00N"/>
+    <hyperlink ref="F32" r:id="rId71" display="SN74LS123N"/>
+    <hyperlink ref="G32" r:id="rId72" display="595-SN74LS123N"/>
+    <hyperlink ref="F33" r:id="rId73" display="74LS157"/>
+    <hyperlink ref="G33" r:id="rId74" display="595-SN74LS157N"/>
+    <hyperlink ref="F34" r:id="rId75" display="SN74LS245N"/>
+    <hyperlink ref="G34" r:id="rId76" display="595-SN74LS245N"/>
+    <hyperlink ref="E36" r:id="rId77" location="" display="30610"/>
+    <hyperlink ref="F36" r:id="rId78" display="ICVT-28P"/>
+    <hyperlink ref="G36" r:id="rId79" display="649-DILB28P223TLF"/>
+    <hyperlink ref="E39" r:id="rId80" location="" display="30605"/>
+    <hyperlink ref="F39" r:id="rId81" display="ICVT-16P"/>
+    <hyperlink ref="E41" r:id="rId82" location="" display="30605"/>
+    <hyperlink ref="F41" r:id="rId83" display="ICVT-16P"/>
+    <hyperlink ref="G42" r:id="rId84" display="595-SN74LS193N"/>
+    <hyperlink ref="F44" r:id="rId85" display="NTE74LS257"/>
+    <hyperlink ref="G44" r:id="rId86" display="595-SN74LS257BN"/>
+    <hyperlink ref="F45" r:id="rId87" display="SN74LS138N"/>
+    <hyperlink ref="G45" r:id="rId88" display="595-SN74LS138N"/>
+    <hyperlink ref="F46" r:id="rId89" display="NTE74LS86"/>
+    <hyperlink ref="G46" r:id="rId90" display="595-SN74LS86AN"/>
+    <hyperlink ref="F47" r:id="rId91" display="NTE74LS95B"/>
+    <hyperlink ref="F48" r:id="rId92" display="AS6C6264-55PIN"/>
+    <hyperlink ref="G48" r:id="rId93" display="913-AS6C6264-55PCN"/>
+    <hyperlink ref="E49" r:id="rId94" location="" display="30610"/>
+    <hyperlink ref="F49" r:id="rId95" display="ICVT-28P"/>
+    <hyperlink ref="G49" r:id="rId96" display="649-DILB28P223TLF"/>
+    <hyperlink ref="E51" r:id="rId97" location="" display="30609"/>
+    <hyperlink ref="F51" r:id="rId98" display="ICVT-24P"/>
+    <hyperlink ref="G51" r:id="rId99" display="649-DILB24P-223TLF"/>
+    <hyperlink ref="F52" r:id="rId100" display="SN74LS20N"/>
+    <hyperlink ref="G52" r:id="rId101" display="595-SN74LS20N"/>
+    <hyperlink ref="F53" r:id="rId102" display="74LS175"/>
+    <hyperlink ref="G53" r:id="rId103" display="595-SN74LS175N"/>
+    <hyperlink ref="F54" r:id="rId104" display="SN74LS153N"/>
+    <hyperlink ref="G54" r:id="rId105" display="595-SN74LS153N"/>
+    <hyperlink ref="E56" r:id="rId106" location="" display="30605"/>
+    <hyperlink ref="F56" r:id="rId107" display="ICVT-16P"/>
+    <hyperlink ref="F57" r:id="rId108" display="74LS174"/>
+    <hyperlink ref="G57" r:id="rId109" display="595-SN74LS174N"/>
+    <hyperlink ref="G58" r:id="rId110" display="595-SN74S04N"/>
+    <hyperlink ref="E59" r:id="rId111" display="17539"/>
+    <hyperlink ref="F59" r:id="rId112" display="SN74HC4066N"/>
+    <hyperlink ref="G59" r:id="rId113" display="595-CD4066BE"/>
+    <hyperlink ref="E63" r:id="rId114" display="19226"/>
+    <hyperlink ref="F63" r:id="rId115" display="DSC-025"/>
+    <hyperlink ref="G63" r:id="rId116" display="710-61802524823"/>
+    <hyperlink ref="E64" r:id="rId117" display="28738"/>
+    <hyperlink ref="F64" r:id="rId118" display="DLA10-N"/>
+    <hyperlink ref="G64" r:id="rId119" display="652-78F100J-TR-RC"/>
+    <hyperlink ref="E68" r:id="rId120" display="30981"/>
+    <hyperlink ref="F68" r:id="rId121" display="CF1/4W-10K"/>
+    <hyperlink ref="G68" r:id="rId122" display="71-CCF0710K0JKE36"/>
+    <hyperlink ref="E69" r:id="rId123" display="30753"/>
+    <hyperlink ref="F69" r:id="rId124" display="CF1/4W-100R"/>
+    <hyperlink ref="G69" r:id="rId125" display="71-CCF07100RJKE36"/>
+    <hyperlink ref="E70" r:id="rId126" display="30848"/>
+    <hyperlink ref="F70" r:id="rId127" display="CF1/4W-680R"/>
+    <hyperlink ref="G70" r:id="rId128" display="71-CCF07680RJKE36"/>
+    <hyperlink ref="E71" r:id="rId129" display="30952"/>
+    <hyperlink ref="F71" r:id="rId130" display="CF1/4W-5K6"/>
+    <hyperlink ref="G71" r:id="rId131" display="71-CCF075K60JKE36"/>
+    <hyperlink ref="F72" r:id="rId132" display="CF1/4W-4K7"/>
+    <hyperlink ref="G72" r:id="rId133" display="71-CCF07-J-4.7K-E3"/>
+    <hyperlink ref="E73" r:id="rId134" display="30789"/>
+    <hyperlink ref="F73" r:id="rId135" display="CF1/4W-220R"/>
+    <hyperlink ref="G73" r:id="rId136" display="71-CCF07220RJKE36"/>
+    <hyperlink ref="E74" r:id="rId137" display="30696"/>
+    <hyperlink ref="F74" r:id="rId138" display="CF1/4W-33R"/>
+    <hyperlink ref="G74" r:id="rId139" display="71-CCF0733R0JKE36"/>
+    <hyperlink ref="E75" r:id="rId140" display="30924"/>
+    <hyperlink ref="F75" r:id="rId141" display="CF1/4W-3K3"/>
+    <hyperlink ref="G75" r:id="rId142" display="71-CCF073K30JKE36"/>
+    <hyperlink ref="F76" r:id="rId143" display="CF1/4W-1K"/>
+    <hyperlink ref="G76" r:id="rId144" display="71-CCF071K00JKE36"/>
+    <hyperlink ref="E77" r:id="rId145" display="30780"/>
+    <hyperlink ref="F77" r:id="rId146" display="CF1/4W-180R"/>
+    <hyperlink ref="G77" r:id="rId147" display="71-CCF07160RJKE36"/>
+    <hyperlink ref="E78" r:id="rId148" display="30933"/>
+    <hyperlink ref="F78" r:id="rId149" display="CF1/4W-3K9"/>
+    <hyperlink ref="G78" r:id="rId150" display="603-CFR-25JB-52-3K9"/>
+    <hyperlink ref="E79" r:id="rId151" display="30829"/>
+    <hyperlink ref="F79" r:id="rId152" display="CF1/4W-470R"/>
+    <hyperlink ref="G79" r:id="rId153" display="71-CCF07470RJKE36"/>
+    <hyperlink ref="E80" r:id="rId154" display="30999"/>
+    <hyperlink ref="F80" r:id="rId155" display="CF1/4W-15K"/>
+    <hyperlink ref="G80" r:id="rId156" display="71-CCF0715K0JKE36"/>
+    <hyperlink ref="E81" r:id="rId157" display="30800"/>
+    <hyperlink ref="F81" r:id="rId158" display="CF1/4W-270R"/>
+    <hyperlink ref="G81" r:id="rId159" display="603-CFR-25JB-52-270R"/>
+    <hyperlink ref="F82" r:id="rId160" display="CF1/4W-2K2"/>
+    <hyperlink ref="G82" r:id="rId161" display="71-CCF072K20JKE36"/>
+    <hyperlink ref="E83" r:id="rId162" display="30871"/>
+    <hyperlink ref="F83" r:id="rId163" display="CF1/4W-1K1"/>
+    <hyperlink ref="G83" r:id="rId164" display="603-CFR-25JR-52-1K1"/>
+    <hyperlink ref="E84" r:id="rId165" display="30734"/>
+    <hyperlink ref="F84" r:id="rId166" display="CF1/4W-68R"/>
+    <hyperlink ref="G84" r:id="rId167" display="71-CCF0768R0JKE36"/>
+    <hyperlink ref="E85" r:id="rId168" display="31028"/>
+    <hyperlink ref="F85" r:id="rId169" display="CF1/4W-27K"/>
+    <hyperlink ref="G85" r:id="rId170" display="603-CFR-25JB-52-27K"/>
+    <hyperlink ref="E86" r:id="rId171" display="30810"/>
+    <hyperlink ref="F86" r:id="rId172" display="CF1/4W-330R"/>
+    <hyperlink ref="G86" r:id="rId173" display="71-CCF07330RJKE36"/>
+    <hyperlink ref="E87" r:id="rId174" display="30857"/>
+    <hyperlink ref="F87" r:id="rId175" display="CF1/4W-820R"/>
+    <hyperlink ref="G87" r:id="rId176" display="71-CCF07820RJKE36"/>
+    <hyperlink ref="F88" r:id="rId177" display="CF1/4W-22R"/>
+    <hyperlink ref="G88" r:id="rId178" display="71-CCF0722R0JKE36"/>
+    <hyperlink ref="E89" r:id="rId179" display="31038"/>
+    <hyperlink ref="F89" r:id="rId180" display="CF1/4W-33K"/>
+    <hyperlink ref="G89" r:id="rId181" display="71-CCF0733K0JKE36"/>
+    <hyperlink ref="E90" r:id="rId182" display="30875"/>
+    <hyperlink ref="F90" r:id="rId183" display="CF1/4W-1K2"/>
+    <hyperlink ref="G90" r:id="rId184" display="603-CFR-25JR-521K2"/>
+    <hyperlink ref="E91" r:id="rId185" display="31209"/>
+    <hyperlink ref="F91" r:id="rId186" display="CF1/4W-1M"/>
+    <hyperlink ref="G91" r:id="rId187" display="71-CCF071M00JKE36"/>
+    <hyperlink ref="E92" r:id="rId188" display="30819"/>
+    <hyperlink ref="F92" r:id="rId189" display="CF1/4W-390R"/>
+    <hyperlink ref="G92" r:id="rId190" display="71-CCF07390RJKE36"/>
+    <hyperlink ref="F93" r:id="rId191" display="4609X-101-102LF"/>
+    <hyperlink ref="G93" r:id="rId192" display="652-4609X-1LF-10K"/>
+    <hyperlink ref="F94" r:id="rId193" display="CA6H-250"/>
+    <hyperlink ref="H95" r:id="rId194" display="pin header, repro odporucam Mouser 497-SM230332-1"/>
+    <hyperlink ref="H101" r:id="rId195" display="jediny zdroj, o ktorom viem, je Farnell 9509488"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4058,6 +4128,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId178"/>
+  <legacyDrawing r:id="rId196"/>
 </worksheet>
 </file>
</xml_diff>